<commit_message>
Update to Blank correction & Mean correction
</commit_message>
<xml_diff>
--- a/res/CheatSheets.xlsx
+++ b/res/CheatSheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbroadhurst/Github/QC-MXP/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B66E413-D1AB-9143-A7A5-C190BA807B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE73EC3-EE28-1147-9BC3-9A68B989EDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2700" windowWidth="27700" windowHeight="16940" activeTab="2" xr2:uid="{D81271CA-93EF-834F-B9E5-659B6E5E8FF3}"/>
+    <workbookView xWindow="4260" yWindow="2700" windowWidth="27700" windowHeight="16940" activeTab="1" xr2:uid="{D81271CA-93EF-834F-B9E5-659B6E5E8FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefilter" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>"Ignore","MPV","NaN"</t>
   </si>
   <si>
-    <t>"Median","Linear","Spline"</t>
-  </si>
-  <si>
     <t>"QC","Reference"</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
   </si>
   <si>
     <t>QC' = both the intra- and inter-batch based on the QC samples; 'Reference' = intra-batch correction based on the QCs but the inter-batch correction uses the samples labelled as 'Reference'.</t>
-  </si>
-  <si>
-    <t>Three correction modes. "Spline" is the default QCRSC algorithm that requires optimisation of the smoothing parameter. "Linear" is a simple (interpolated) linear regression based on the QC values &amp; as such requires no smoothing optimisation. "Median" equalises the QC median across batches &amp; ignores within batch systematic change.</t>
   </si>
   <si>
     <t>The 'linear'/quadratic/cubic' options fit a simple polynomial function to the QC data using robust least squares regression. Points outside the population confidence interval are deemed outliers. The 'percentile' option implements the standard non-parametric &lt;  Q1 − 1.5 IQR or  &gt; Q3 + 1.5 IQR outlier detection method on the QC samples.</t>
@@ -309,6 +303,12 @@
   </si>
   <si>
     <t>PCA model is generated using only the Sample data. This removes any possible bias from the QC, Blank, or Reference samples. The QC, Blank, or Reference sample data can applied to the PCA model (projected through) and plotted with the Sample data.</t>
+  </si>
+  <si>
+    <t>"Mean","Linear","Spline"</t>
+  </si>
+  <si>
+    <t>Three correction modes. "Spline" is the default QCRSC algorithm that requires optimisation of the smoothing parameter. "Linear" is a simple (interpolated) linear regression based on the QC values &amp; as such requires no smoothing optimisation. "Mean" equalises the QC mean across batches &amp; ignores within batch systematic change.</t>
   </si>
 </sst>
 </file>
@@ -661,32 +661,32 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,16 +1034,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>1</v>
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1440AF-6D0E-2548-A770-1EACB8A69641}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="107" workbookViewId="0">
-      <selection sqref="A1:C17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="107" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1086,14 +1086,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="40" x14ac:dyDescent="0.25">
@@ -1115,7 +1115,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="40" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="40" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1167,10 +1167,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1178,10 +1178,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="80" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="40" x14ac:dyDescent="0.25">
@@ -1200,10 +1200,10 @@
         <v>16</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="80" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>30</v>
@@ -1233,10 +1233,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>33</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="80" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
         <v>34</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="41" thickBot="1" x14ac:dyDescent="0.3">
@@ -1282,7 +1282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14340D4-650A-D548-A81E-733CEBC5D446}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B18"/>
     </sheetView>
   </sheetViews>
@@ -1293,136 +1293,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>43</v>
+      <c r="B1" s="31" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" ht="40" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="25"/>
     </row>
     <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="25"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="29"/>
+        <v>69</v>
+      </c>
+      <c r="B17" s="37"/>
     </row>
     <row r="18" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="31"/>
+      <c r="A18" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update docs for version 1.1
</commit_message>
<xml_diff>
--- a/res/CheatSheets.xlsx
+++ b/res/CheatSheets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbroadhurst/Github/QC-MXP/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvdbrdhrst/GitHub/QC-MXP/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE73EC3-EE28-1147-9BC3-9A68B989EDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F14B56B-0285-F94E-9708-48D6517BB1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2700" windowWidth="27700" windowHeight="16940" activeTab="1" xr2:uid="{D81271CA-93EF-834F-B9E5-659B6E5E8FF3}"/>
+    <workbookView xWindow="4260" yWindow="2700" windowWidth="27700" windowHeight="16940" activeTab="2" xr2:uid="{D81271CA-93EF-834F-B9E5-659B6E5E8FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefilter" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
   <si>
     <t>☒  Batch-wise</t>
   </si>
@@ -67,9 +67,6 @@
     <t>RemoveZeros</t>
   </si>
   <si>
-    <t>OutlierScope</t>
-  </si>
-  <si>
     <t>OutlierMethod</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>"None","Percentile","Linear","Quadratic","Cubic"</t>
   </si>
   <si>
-    <t>"Local","Global", "Global&amp;Local"</t>
-  </si>
-  <si>
     <t>value between between 0.9 and 0.99</t>
   </si>
   <si>
@@ -169,9 +163,6 @@
     <t>Explanation</t>
   </si>
   <si>
-    <t>Perform outlier detection per batch, across all the batches, or both</t>
-  </si>
-  <si>
     <t>Choose whether summary statistics for each corrected feature are calculated using parametric (mean, standard deviation etc) or non-parametric methods (median, median absolute deviation etc).</t>
   </si>
   <si>
@@ -251,9 +242,6 @@
   </si>
   <si>
     <t>Project in Reference samples</t>
-  </si>
-  <si>
-    <t>Should the filter bank calculate its statistics across all batches or calulate each batch individually and select the worst batch to represent that peak.</t>
   </si>
   <si>
     <t>% allowed missing samples. e.g. if 20% then peak is removed if number of missing &gt; 20%.</t>
@@ -308,7 +296,10 @@
     <t>"Mean","Linear","Spline"</t>
   </si>
   <si>
-    <t>Three correction modes. "Spline" is the default QCRSC algorithm that requires optimisation of the smoothing parameter. "Linear" is a simple (interpolated) linear regression based on the QC values &amp; as such requires no smoothing optimisation. "Mean" equalises the QC mean across batches &amp; ignores within batch systematic change.</t>
+    <t>Three correction modes. "Spline" is the default QCRSC algorithm that requires optimisation of the smoothing parameter. "Linear" is a simple Robust (bisquare) linear regression based on the QC values &amp; requires no smoothing optimisation. "Mean" equalises the QC mean across batches &amp; ignores within batch systematic change.</t>
+  </si>
+  <si>
+    <t>Should the filter bank calculate its peak-wise statistics across all batches or calulate each batch individually and then summarise based on the dropdown option (e.g. "Mean" = the mean of all the batch statistics &amp; "Max" = the poorest statistic comparing all batches).</t>
   </si>
 </sst>
 </file>
@@ -585,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -625,9 +616,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -1034,34 +1022,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1072,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1440AF-6D0E-2548-A770-1EACB8A69641}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="107" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A13" zoomScale="107" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1086,14 +1074,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>42</v>
+      <c r="A1" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="40" x14ac:dyDescent="0.25">
@@ -1101,10 +1089,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="40" x14ac:dyDescent="0.25">
@@ -1112,24 +1100,24 @@
         <v>8</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="40" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>26</v>
+      <c r="B4" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="40" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
@@ -1137,139 +1125,128 @@
         <v>25</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="40" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="80" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="80" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="40" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="40" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="80" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="80" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="140" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="140" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="80" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="80" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="41" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="17" t="s">
         <v>32</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1282,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14340D4-650A-D548-A81E-733CEBC5D446}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1293,136 +1270,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>42</v>
+      <c r="A1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" ht="40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="80" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>76</v>
+      <c r="A7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>75</v>
+      <c r="A8" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>74</v>
+      <c r="A9" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="B15" s="24"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="25"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="37"/>
+      <c r="B17" s="36"/>
     </row>
     <row r="18" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="38"/>
+      <c r="A18" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>